<commit_message>
Printed Logs to Python Terminal
</commit_message>
<xml_diff>
--- a/Timetable.xlsx
+++ b/Timetable.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="312" yWindow="672" windowWidth="17280" windowHeight="8964" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8964" windowWidth="17280" xWindow="312" yWindow="672"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -59,31 +59,31 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -396,11 +396,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="17.77734375" customWidth="1" style="4" min="1" max="1"/>
-    <col width="11.109375" customWidth="1" style="4" min="2" max="4"/>
-    <col width="10.77734375" customWidth="1" style="4" min="5" max="10"/>
-    <col width="11.109375" customWidth="1" style="4" min="11" max="19"/>
-    <col width="10.77734375" customWidth="1" style="4" min="20" max="21"/>
+    <col customWidth="1" max="1" min="1" style="4" width="17.77734375"/>
+    <col customWidth="1" max="4" min="2" style="4" width="11.109375"/>
+    <col customWidth="1" max="10" min="5" style="4" width="10.77734375"/>
+    <col customWidth="1" max="19" min="11" style="4" width="11.109375"/>
+    <col customWidth="1" max="21" min="20" style="4" width="10.77734375"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -558,17 +558,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
+          <t>B Tech IT</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>B Tech IT</t>
+          <t>MBA Tech CS</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>MBA Tech CS</t>
+          <t>MBA Tech IT</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -583,66 +583,74 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>MBA Tech CS</t>
+          <t>MBA Tech IT</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
+          <t>MBA Tech CS</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
+          <t>MBA Tech CS</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>B Tech CS</t>
+          <t>MBA Tech IT</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>B Tech IT</t>
+          <t>B Tech CS</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>MBA Tech CS</t>
+          <t>B Tech IT</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>B Tech CS</t>
+          <t>MBA Tech IT</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
+          <t>MBA Tech CS</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>MBA Tech CS</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr"/>
+          <t>B Tech IT</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>B Tech CS</t>
+        </is>
+      </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>B Tech IT</t>
+          <t>B Tech CS</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>B Tech CS</t>
+          <t>B Tech IT</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr"/>
+          <t>MBA Tech CS</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>MBA Tech IT</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -652,7 +660,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
+          <t>B Tech IT</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -662,13 +670,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>B Tech IT</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
+          <t>MBA Tech IT</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>MBA Tech CS</t>
+        </is>
+      </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>B Tech CS</t>
+          <t>MBA Tech CS</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -678,23 +690,27 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>MBA Tech CS</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr"/>
+          <t>B Tech CS</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>B Tech IT</t>
+        </is>
+      </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>B Tech IT</t>
+          <t>MBA Tech IT</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
+          <t>MBA Tech CS</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>MBA Tech CS</t>
+          <t>B Tech IT</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
@@ -704,40 +720,44 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
+          <t>B Tech CS</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>B Tech CS</t>
+          <t>B Tech IT</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>B Tech IT</t>
+          <t>MBA Tech CS</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>MBA Tech CS</t>
+          <t>MBA Tech IT</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>B Tech CS</t>
+          <t>B Tech IT</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
+          <t>B Tech CS</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>B Tech IT</t>
-        </is>
-      </c>
-      <c r="U5" t="inlineStr"/>
+          <t>MBA Tech IT</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>MBA Tech CS</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -747,20 +767,24 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>B Tech IT</t>
+          <t>MBA Tech CS</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>B Tech CS</t>
+          <t>MBA Tech IT</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
+          <t>B Tech CS</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>B Tech IT</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
           <t>MBA Tech IT</t>
@@ -768,15 +792,19 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>B Tech CS</t>
+          <t>MBA Tech CS</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>MBA Tech CS</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr"/>
+          <t>B Tech IT</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>B Tech CS</t>
+        </is>
+      </c>
       <c r="J6" t="inlineStr">
         <is>
           <t>B Tech CS</t>
@@ -784,15 +812,19 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
+          <t>B Tech IT</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>B Tech IT</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr"/>
+          <t>MBA Tech CS</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>MBA Tech IT</t>
+        </is>
+      </c>
       <c r="N6" t="inlineStr">
         <is>
           <t>B Tech IT</t>
@@ -800,31 +832,39 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
+          <t>B Tech CS</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>MBA Tech CS</t>
+          <t>MBA Tech IT</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>B Tech CS</t>
+          <t>MBA Tech CS</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
+          <t>MBA Tech CS</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>B Tech CS</t>
-        </is>
-      </c>
-      <c r="T6" t="inlineStr"/>
-      <c r="U6" t="inlineStr"/>
+          <t>MBA Tech IT</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>B Tech CS</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>B Tech IT</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -834,64 +874,104 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>B Tech CS</t>
+          <t>MBA Tech IT</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+          <t>MBA Tech CS</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>B Tech IT</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>B Tech CS</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
+          <t>B Tech CS</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>B Tech CS</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
+          <t>B Tech IT</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>MBA Tech CS</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>MBA Tech IT</t>
+        </is>
+      </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>B Tech CS</t>
+          <t>B Tech IT</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
+          <t>B Tech CS</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>MBA Tech IT</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>MBA Tech CS</t>
+        </is>
+      </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
+          <t>MBA Tech CS</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>B Tech CS</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
+          <t>MBA Tech IT</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>B Tech CS</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>B Tech IT</t>
+        </is>
+      </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>B Tech CS</t>
+          <t>MBA Tech IT</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
-        </is>
-      </c>
-      <c r="T7" t="inlineStr"/>
-      <c r="U7" t="inlineStr"/>
+          <t>MBA Tech CS</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>B Tech IT</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>B Tech CS</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -913,62 +993,94 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
+          <t>B Tech CS</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>B Tech CS</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
+          <t>B Tech IT</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>MBA Tech CS</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>MBA Tech IT</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>B Tech CS</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr"/>
+          <t>B Tech IT</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>B Tech CS</t>
+        </is>
+      </c>
       <c r="H9" t="inlineStr">
         <is>
           <t>MBA Tech IT</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr"/>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>MBA Tech CS</t>
+        </is>
+      </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
+          <t>MBA Tech CS</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>B Tech CS</t>
+          <t>MBA Tech IT</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>B Tech IT</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr"/>
+          <t>B Tech CS</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>B Tech IT</t>
+        </is>
+      </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>B Tech CS</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr"/>
+          <t>MBA Tech IT</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>MBA Tech CS</t>
+        </is>
+      </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
-        </is>
-      </c>
-      <c r="Q9" t="inlineStr"/>
+          <t>B Tech IT</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>B Tech CS</t>
+        </is>
+      </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
-        </is>
-      </c>
-      <c r="S9" t="inlineStr"/>
+          <t>B Tech CS</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>B Tech IT</t>
+        </is>
+      </c>
       <c r="T9" t="inlineStr">
         <is>
           <t>MBA Tech CS</t>
@@ -976,7 +1088,7 @@
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>B Tech CS</t>
+          <t>MBA Tech IT</t>
         </is>
       </c>
     </row>
@@ -988,63 +1100,99 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr"/>
+          <t>B Tech IT</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>B Tech CS</t>
+        </is>
+      </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>B Tech IT</t>
+          <t>MBA Tech IT</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>B Tech CS</t>
+          <t>MBA Tech CS</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr"/>
+          <t>MBA Tech CS</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>MBA Tech IT</t>
+        </is>
+      </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>MBA Tech CS</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr"/>
+          <t>B Tech CS</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>B Tech IT</t>
+        </is>
+      </c>
       <c r="J10" t="inlineStr">
         <is>
           <t>MBA Tech IT</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>MBA Tech CS</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>B Tech IT</t>
+        </is>
+      </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>MBA Tech CS</t>
+          <t>B Tech CS</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
+          <t>B Tech CS</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>B Tech IT</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>MBA Tech CS</t>
+        </is>
+      </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>B Tech CS</t>
+          <t>MBA Tech IT</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
-        </is>
-      </c>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="inlineStr"/>
+          <t>B Tech IT</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>B Tech CS</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>MBA Tech IT</t>
+        </is>
+      </c>
       <c r="U10" t="inlineStr">
         <is>
           <t>MBA Tech CS</t>
@@ -1059,44 +1207,104 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
+          <t>MBA Tech CS</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>MBA Tech IT</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>B Tech CS</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>B Tech IT</t>
+        </is>
+      </c>
       <c r="F11" t="inlineStr">
         <is>
           <t>MBA Tech IT</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>MBA Tech CS</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>B Tech IT</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>B Tech CS</t>
+        </is>
+      </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
+          <t>B Tech CS</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>B Tech IT</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>MBA Tech CS</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>MBA Tech IT</t>
+        </is>
+      </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr"/>
+          <t>B Tech IT</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>B Tech CS</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>MBA Tech IT</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>MBA Tech CS</t>
+        </is>
+      </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
-        </is>
-      </c>
-      <c r="S11" t="inlineStr"/>
-      <c r="T11" t="inlineStr"/>
-      <c r="U11" t="inlineStr"/>
+          <t>MBA Tech CS</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>MBA Tech IT</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>B Tech CS</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>B Tech IT</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1104,50 +1312,58 @@
           <t>4:00 pm - 5:00 pm</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>MBA Tech IT</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>MBA Tech CS</t>
+        </is>
+      </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>MBA Tech IT</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
+          <t>B Tech IT</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>B Tech CS</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>B Tech CS</t>
+        </is>
+      </c>
       <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>MBA Tech IT</t>
-        </is>
-      </c>
+      <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>B Tech CS</t>
+        </is>
+      </c>
       <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>MBA Tech IT</t>
-        </is>
-      </c>
+      <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>B Tech CS</t>
+        </is>
+      </c>
       <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr">
-        <is>
-          <t>MBA Tech IT</t>
-        </is>
-      </c>
+      <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr"/>
-      <c r="R12" t="inlineStr"/>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>B Tech CS</t>
+        </is>
+      </c>
       <c r="S12" t="inlineStr"/>
-      <c r="T12" t="inlineStr">
-        <is>
-          <t>B Tech IT</t>
-        </is>
-      </c>
-      <c r="U12" t="inlineStr">
-        <is>
-          <t>MBA Tech IT</t>
-        </is>
-      </c>
+      <c r="T12" t="inlineStr"/>
+      <c r="U12" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1160,7 +1376,7 @@
     <mergeCell ref="R2:U2"/>
     <mergeCell ref="B1:U1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>